<commit_message>
"Textures halved and birds cut only for what is used. Time to set final bird flight patterns and create UI, then finish assets. also remember gold coin not spinning bug"
</commit_message>
<xml_diff>
--- a/android/assets/flockBlockersExtra/spec.xlsx
+++ b/android/assets/flockBlockersExtra/spec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>(Fast Firing)</t>
   </si>
@@ -159,15 +159,9 @@
     <t>X</t>
   </si>
   <si>
-    <t>1 diamond=10000 gold</t>
-  </si>
-  <si>
     <t>1000 diamonds</t>
   </si>
   <si>
-    <t>500 diamonds</t>
-  </si>
-  <si>
     <t>???</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     <t>Size</t>
   </si>
   <si>
-    <t>Amount (*1.1 each time up to 3x original amounts, then health x2 (&amp;goldx2.5) until 10x original)</t>
-  </si>
-  <si>
     <t>Dmg</t>
   </si>
   <si>
@@ -256,6 +247,33 @@
   </si>
   <si>
     <t>7+Diamond</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>3000 diamonds</t>
+  </si>
+  <si>
+    <t>10000 diamonds</t>
+  </si>
+  <si>
+    <t>90c/1000 0.09c/dia</t>
+  </si>
+  <si>
+    <t>$5/10000 0.05c/dia</t>
+  </si>
+  <si>
+    <t>$2/3000 0.07c/dia</t>
+  </si>
+  <si>
+    <t>90c/no ads</t>
+  </si>
+  <si>
+    <t>Amount (*1.15 each time up to 3x original amounts, then health x2 (&amp;goldx2.5) until 10x original)</t>
+  </si>
+  <si>
+    <t>1 dia=1000 go, 5000 go=1 dia</t>
   </si>
 </sst>
 </file>
@@ -625,52 +643,70 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="2">
+        <v>500</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4500</v>
+      </c>
+      <c r="E2" s="2">
+        <v>13500</v>
+      </c>
+      <c r="F2" s="2">
+        <v>40500</v>
+      </c>
+      <c r="G2" s="2">
+        <v>121500</v>
+      </c>
+      <c r="H2" s="2">
+        <v>364500</v>
+      </c>
+      <c r="I2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="2">
-        <v>500</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2000</v>
-      </c>
-      <c r="E2" s="2">
-        <v>8000</v>
-      </c>
-      <c r="F2" s="2">
-        <v>32000</v>
-      </c>
-      <c r="G2" s="2">
-        <v>128000</v>
-      </c>
-      <c r="H2" s="2">
-        <v>512000</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2048000</v>
-      </c>
-      <c r="J2" t="s">
-        <v>49</v>
+      <c r="J2" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -725,7 +761,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -746,7 +782,7 @@
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L4" s="1">
         <v>2</v>
@@ -769,7 +805,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -790,7 +826,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L5" s="1">
         <v>4</v>
@@ -813,7 +849,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -834,7 +870,7 @@
         <v>8</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
@@ -851,50 +887,50 @@
     </row>
     <row r="8" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>62</v>
       </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
-      </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <v>40</v>
@@ -902,16 +938,16 @@
     </row>
     <row r="12" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -922,16 +958,16 @@
     </row>
     <row r="13" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E13">
         <v>15</v>
@@ -942,16 +978,16 @@
     </row>
     <row r="14" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E14">
         <v>15</v>
@@ -962,16 +998,16 @@
     </row>
     <row r="15" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -982,16 +1018,16 @@
     </row>
     <row r="16" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E16">
         <v>50</v>
@@ -1002,16 +1038,16 @@
     </row>
     <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1">
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -1022,19 +1058,19 @@
     </row>
     <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1">
         <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G18">
         <v>1</v>

</xml_diff>